<commit_message>
Vorabversion der JSON-Schnittstellen - englische Bezeichner - Versionsnummer - englischer Vorlesungsbezeichnung wird durch Deutsche ersetzt, sollte diese fehlen - Nur Semester des der aktuellen Periode (SS/WS) werde angezeigt. - MSchedule liefert zusammengeführtes JSON um direkt die Änderungen zu erhalten.
</commit_message>
<xml_diff>
--- a/Spaltennamen.xlsx
+++ b/Spaltennamen.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965"/>
   </bookViews>
   <sheets>
-    <sheet name="Studiengaenge" sheetId="1" r:id="rId1"/>
-    <sheet name="Stundenplan_WWW" sheetId="2" r:id="rId2"/>
-    <sheet name="Verlegungnen_WWW" sheetId="3" r:id="rId3"/>
+    <sheet name="Schnittstelle" sheetId="4" r:id="rId1"/>
+    <sheet name="Studiengaenge" sheetId="1" r:id="rId2"/>
+    <sheet name="Stundenplan_WWW" sheetId="2" r:id="rId3"/>
+    <sheet name="Verlegungnen_WWW" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="170">
   <si>
     <t>id</t>
   </si>
@@ -423,6 +424,114 @@
   </si>
   <si>
     <t>Raum für den neuen Termin</t>
+  </si>
+  <si>
+    <t>stgnr</t>
+  </si>
+  <si>
+    <t>de</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>semester</t>
+  </si>
+  <si>
+    <t>period</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>dozent</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>weekday</t>
+  </si>
+  <si>
+    <t>room</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>name (überflüssig?)</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>reason</t>
+  </si>
+  <si>
+    <t>schedule_id</t>
+  </si>
+  <si>
+    <t>labels</t>
+  </si>
+  <si>
+    <t>Studiengänge</t>
+  </si>
+  <si>
+    <t>Tabelle</t>
+  </si>
+  <si>
+    <t>Stundenplan_WWW</t>
+  </si>
+  <si>
+    <t>splusname</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>docent</t>
+  </si>
+  <si>
+    <t>stattime, startdate</t>
+  </si>
+  <si>
+    <t>endtime, enddate</t>
+  </si>
+  <si>
+    <t>Es werden 2 Felder nach den folgenden Munstern  erzeugt: (HH:mm) (dd.mm.YYYY)</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>Verlegungen_WWW</t>
+  </si>
+  <si>
+    <t>original</t>
+  </si>
+  <si>
+    <t>time, date</t>
+  </si>
+  <si>
+    <t>alternative</t>
+  </si>
+  <si>
+    <t>Objekt das die Ersatzdaten enthält</t>
+  </si>
+  <si>
+    <t>Objekt das die Ausfalldaten enthält</t>
+  </si>
+  <si>
+    <t>Zusammengeführter Stundenplan</t>
+  </si>
+  <si>
+    <t>changes</t>
+  </si>
+  <si>
+    <t>Objekt welches die Änderungen enthält oder null liefert</t>
   </si>
 </sst>
 </file>
@@ -430,9 +539,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="172" formatCode="dd\-mmm\-yy"/>
+    <numFmt numFmtId="164" formatCode="dd\-mmm\-yy"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -460,16 +569,52 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -492,13 +637,246 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -507,10 +885,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -518,17 +892,82 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Eingabe" xfId="3" builtinId="20"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard_Tabelle1" xfId="1"/>
     <cellStyle name="Standard_Verlegungnen_WWW" xfId="2"/>
@@ -843,28 +1282,866 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="75.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35" customWidth="1"/>
+    <col min="7" max="7" width="24.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="23"/>
+      <c r="G2" s="24"/>
+    </row>
+    <row r="3" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="48" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3" s="49"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="27"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="51"/>
+      <c r="B4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="52" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" s="42"/>
+      <c r="E4" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="29"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="51"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="53" t="s">
+        <v>150</v>
+      </c>
+      <c r="D5" s="42"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="29"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="51"/>
+      <c r="B6" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="53" t="s">
+        <v>135</v>
+      </c>
+      <c r="D6" s="42"/>
+      <c r="E6" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="29"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="51"/>
+      <c r="B7" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="53" t="s">
+        <v>136</v>
+      </c>
+      <c r="D7" s="42"/>
+      <c r="E7" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="11"/>
+      <c r="G7" s="29"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="51"/>
+      <c r="B8" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="54" t="s">
+        <v>137</v>
+      </c>
+      <c r="D8" s="42"/>
+      <c r="E8" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="11"/>
+      <c r="G8" s="29"/>
+    </row>
+    <row r="9" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="30"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="30"/>
+      <c r="G9" s="31"/>
+    </row>
+    <row r="10" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="B10" s="49"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="27"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="51"/>
+      <c r="B11" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="52" t="s">
+        <v>156</v>
+      </c>
+      <c r="D11" s="42"/>
+      <c r="E11" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" s="32" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="51"/>
+      <c r="B12" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="52" t="s">
+        <v>160</v>
+      </c>
+      <c r="D12" s="42"/>
+      <c r="E12" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12" s="32" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="51"/>
+      <c r="B13" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="52" t="s">
+        <v>145</v>
+      </c>
+      <c r="D13" s="42"/>
+      <c r="E13" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G13" s="32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="51"/>
+      <c r="B14" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="52" t="s">
+        <v>142</v>
+      </c>
+      <c r="D14" s="42"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" s="32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="51"/>
+      <c r="B15" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="52" t="s">
+        <v>157</v>
+      </c>
+      <c r="D15" s="42" t="s">
+        <v>159</v>
+      </c>
+      <c r="E15" s="28"/>
+      <c r="F15" s="11">
+        <v>42460.333333333336</v>
+      </c>
+      <c r="G15" s="29">
+        <v>42489.40625</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="51"/>
+      <c r="B16" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="52" t="s">
+        <v>158</v>
+      </c>
+      <c r="D16" s="42" t="s">
+        <v>159</v>
+      </c>
+      <c r="E16" s="28"/>
+      <c r="F16" s="11">
+        <v>42726.395833333336</v>
+      </c>
+      <c r="G16" s="29">
+        <v>42489.71875</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="51"/>
+      <c r="B17" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="52" t="s">
+        <v>155</v>
+      </c>
+      <c r="D17" s="42"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G17" s="32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="51"/>
+      <c r="B18" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="52" t="s">
+        <v>144</v>
+      </c>
+      <c r="D18" s="42"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="G18" s="33" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="51"/>
+      <c r="B19" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="52" t="s">
+        <v>154</v>
+      </c>
+      <c r="D19" s="42"/>
+      <c r="E19" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="G19" s="34" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="30"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="30"/>
+      <c r="G20" s="31"/>
+    </row>
+    <row r="21" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="48" t="s">
+        <v>161</v>
+      </c>
+      <c r="B21" s="49"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="27"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="51"/>
+      <c r="B22" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="52" t="s">
+        <v>160</v>
+      </c>
+      <c r="D22" s="42"/>
+      <c r="E22" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="G22" s="29"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="51"/>
+      <c r="B23" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="52" t="s">
+        <v>156</v>
+      </c>
+      <c r="D23" s="42"/>
+      <c r="E23" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G23" s="29"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="51"/>
+      <c r="B24" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="52" t="s">
+        <v>147</v>
+      </c>
+      <c r="D24" s="42"/>
+      <c r="E24" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="G24" s="29"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="51"/>
+      <c r="B25" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" s="52" t="s">
+        <v>148</v>
+      </c>
+      <c r="D25" s="42"/>
+      <c r="E25" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="G25" s="29"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="51"/>
+      <c r="B26" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="52" t="s">
+        <v>142</v>
+      </c>
+      <c r="D26" s="42"/>
+      <c r="E26" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="G26" s="29"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="51"/>
+      <c r="B27" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="C27" s="52" t="s">
+        <v>154</v>
+      </c>
+      <c r="D27" s="42"/>
+      <c r="E27" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="G27" s="29"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="51"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="53" t="s">
+        <v>162</v>
+      </c>
+      <c r="D28" s="42" t="s">
+        <v>166</v>
+      </c>
+      <c r="E28" s="28"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="29"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="51"/>
+      <c r="B29" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="53" t="s">
+        <v>155</v>
+      </c>
+      <c r="D29" s="42"/>
+      <c r="E29" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G29" s="29"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="51"/>
+      <c r="B30" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" s="53" t="s">
+        <v>163</v>
+      </c>
+      <c r="D30" s="42" t="s">
+        <v>159</v>
+      </c>
+      <c r="E30" s="28">
+        <v>42299.583333333336</v>
+      </c>
+      <c r="F30" s="7">
+        <v>42285.333333333336</v>
+      </c>
+      <c r="G30" s="29"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="51"/>
+      <c r="B31" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="53" t="s">
+        <v>144</v>
+      </c>
+      <c r="D31" s="42"/>
+      <c r="E31" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="G31" s="29"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="51"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="54" t="s">
+        <v>164</v>
+      </c>
+      <c r="D32" s="42" t="s">
+        <v>165</v>
+      </c>
+      <c r="E32" s="28"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="29"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="51"/>
+      <c r="B33" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" s="54" t="s">
+        <v>155</v>
+      </c>
+      <c r="D33" s="42"/>
+      <c r="E33" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G33" s="29"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="51"/>
+      <c r="B34" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C34" s="54" t="s">
+        <v>163</v>
+      </c>
+      <c r="D34" s="42" t="s">
+        <v>159</v>
+      </c>
+      <c r="E34" s="28">
+        <v>42297.729166666664</v>
+      </c>
+      <c r="F34" s="7">
+        <v>42286.333333333336</v>
+      </c>
+      <c r="G34" s="29"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="51"/>
+      <c r="B35" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C35" s="54" t="s">
+        <v>144</v>
+      </c>
+      <c r="D35" s="42"/>
+      <c r="E35" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="G35" s="29"/>
+    </row>
+    <row r="36" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="35"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="44"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="36"/>
+    </row>
+    <row r="37" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="48" t="s">
+        <v>167</v>
+      </c>
+      <c r="B37" s="49"/>
+      <c r="C37" s="50"/>
+      <c r="D37" s="41"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="27"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="51"/>
+      <c r="B38" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="52" t="s">
+        <v>160</v>
+      </c>
+      <c r="D38" s="42"/>
+      <c r="E38" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G38" s="32" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="51"/>
+      <c r="B39" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C39" s="52" t="s">
+        <v>156</v>
+      </c>
+      <c r="D39" s="42"/>
+      <c r="E39" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G39" s="32" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="51"/>
+      <c r="B40" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" s="52" t="s">
+        <v>145</v>
+      </c>
+      <c r="D40" s="42"/>
+      <c r="E40" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G40" s="32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="51"/>
+      <c r="B41" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41" s="52" t="s">
+        <v>142</v>
+      </c>
+      <c r="D41" s="42"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G41" s="32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="51"/>
+      <c r="B42" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C42" s="52" t="s">
+        <v>157</v>
+      </c>
+      <c r="D42" s="42" t="s">
+        <v>159</v>
+      </c>
+      <c r="E42" s="28"/>
+      <c r="F42" s="11">
+        <v>42460.333333333336</v>
+      </c>
+      <c r="G42" s="29">
+        <v>42489.40625</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="51"/>
+      <c r="B43" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C43" s="52" t="s">
+        <v>158</v>
+      </c>
+      <c r="D43" s="42" t="s">
+        <v>159</v>
+      </c>
+      <c r="E43" s="28"/>
+      <c r="F43" s="11">
+        <v>42726.395833333336</v>
+      </c>
+      <c r="G43" s="29">
+        <v>42489.71875</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="51"/>
+      <c r="B44" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44" s="52" t="s">
+        <v>155</v>
+      </c>
+      <c r="D44" s="42"/>
+      <c r="E44" s="28"/>
+      <c r="F44" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G44" s="32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="51"/>
+      <c r="B45" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C45" s="52" t="s">
+        <v>144</v>
+      </c>
+      <c r="D45" s="42"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="G45" s="33" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="51"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="54" t="s">
+        <v>168</v>
+      </c>
+      <c r="D46" s="42" t="s">
+        <v>169</v>
+      </c>
+      <c r="E46" s="28"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="34"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="51"/>
+      <c r="B47" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47" s="54" t="s">
+        <v>147</v>
+      </c>
+      <c r="D47" s="42"/>
+      <c r="E47" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="G47" s="29"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="51"/>
+      <c r="B48" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C48" s="54" t="s">
+        <v>148</v>
+      </c>
+      <c r="D48" s="42"/>
+      <c r="E48" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="G48" s="29"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="51"/>
+      <c r="B49" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C49" s="54" t="s">
+        <v>155</v>
+      </c>
+      <c r="D49" s="42"/>
+      <c r="E49" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G49" s="29"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="51"/>
+      <c r="B50" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C50" s="54" t="s">
+        <v>163</v>
+      </c>
+      <c r="D50" s="42" t="s">
+        <v>159</v>
+      </c>
+      <c r="E50" s="28">
+        <v>42297.729166666664</v>
+      </c>
+      <c r="F50" s="7">
+        <v>42286.333333333336</v>
+      </c>
+      <c r="G50" s="29"/>
+    </row>
+    <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="55"/>
+      <c r="B51" s="56" t="s">
+        <v>95</v>
+      </c>
+      <c r="C51" s="57" t="s">
+        <v>144</v>
+      </c>
+      <c r="D51" s="45"/>
+      <c r="E51" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="F51" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="G51" s="39"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="39.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="10"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="8"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -878,81 +2155,111 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
       <c r="D3">
         <v>490</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
+      <c r="B4" t="s">
+        <v>134</v>
+      </c>
       <c r="D4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
       <c r="D5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
+      <c r="B6" t="s">
+        <v>135</v>
+      </c>
       <c r="D6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
+      <c r="B7" t="s">
+        <v>136</v>
+      </c>
       <c r="D7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
       <c r="D8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
+      <c r="B9" t="s">
+        <v>59</v>
+      </c>
       <c r="D9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
+      <c r="B10" t="s">
+        <v>59</v>
+      </c>
       <c r="D10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
+      <c r="B11" t="s">
+        <v>59</v>
+      </c>
       <c r="D11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>59</v>
       </c>
       <c r="D12" t="s">
         <v>18</v>
@@ -967,31 +2274,31 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="10"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="8"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -1001,16 +2308,19 @@
       <c r="C2" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
       <c r="D3">
         <v>1237361</v>
       </c>
@@ -1021,10 +2331,13 @@
         <v>1331587</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
+      <c r="B4" t="s">
+        <v>134</v>
+      </c>
       <c r="D4" t="s">
         <v>49</v>
       </c>
@@ -1035,10 +2348,13 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
+      <c r="B5" t="s">
+        <v>137</v>
+      </c>
       <c r="D5" t="s">
         <v>50</v>
       </c>
@@ -1049,10 +2365,13 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
+      <c r="B6" t="s">
+        <v>138</v>
+      </c>
       <c r="D6" t="s">
         <v>51</v>
       </c>
@@ -1063,10 +2382,13 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
+      <c r="B7" t="s">
+        <v>139</v>
+      </c>
       <c r="D7">
         <v>2016</v>
       </c>
@@ -1077,10 +2399,13 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
       <c r="E8" s="3" t="s">
         <v>65</v>
       </c>
@@ -1088,10 +2413,13 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
+      <c r="B9" t="s">
+        <v>59</v>
+      </c>
       <c r="D9" t="s">
         <v>52</v>
       </c>
@@ -1102,10 +2430,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>24</v>
       </c>
+      <c r="B10" t="s">
+        <v>59</v>
+      </c>
       <c r="D10" t="s">
         <v>53</v>
       </c>
@@ -1116,10 +2447,13 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>25</v>
       </c>
+      <c r="B11" t="s">
+        <v>59</v>
+      </c>
       <c r="D11" t="s">
         <v>54</v>
       </c>
@@ -1130,10 +2464,13 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
+      <c r="B12" t="s">
+        <v>59</v>
+      </c>
       <c r="D12" t="s">
         <v>55</v>
       </c>
@@ -1144,10 +2481,13 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
+      <c r="B13" t="s">
+        <v>140</v>
+      </c>
       <c r="D13" t="s">
         <v>56</v>
       </c>
@@ -1158,10 +2498,13 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
+      <c r="B14" t="s">
+        <v>141</v>
+      </c>
       <c r="D14" t="s">
         <v>57</v>
       </c>
@@ -1172,10 +2515,13 @@
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
+      <c r="B15" t="s">
+        <v>59</v>
+      </c>
       <c r="D15" t="s">
         <v>58</v>
       </c>
@@ -1186,10 +2532,13 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>29</v>
       </c>
+      <c r="B16" t="s">
+        <v>59</v>
+      </c>
       <c r="E16" s="3" t="s">
         <v>65</v>
       </c>
@@ -1197,10 +2546,13 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>30</v>
       </c>
+      <c r="B17" t="s">
+        <v>59</v>
+      </c>
       <c r="D17" t="s">
         <v>59</v>
       </c>
@@ -1211,10 +2563,13 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>31</v>
       </c>
+      <c r="B18" t="s">
+        <v>142</v>
+      </c>
       <c r="E18" s="3" t="s">
         <v>72</v>
       </c>
@@ -1222,100 +2577,136 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="4">
-        <v>42460.333333333336</v>
-      </c>
-      <c r="F19" s="4">
-        <v>42489.40625</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+      <c r="B19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" s="4">
-        <v>42726.395833333336</v>
-      </c>
-      <c r="F20" s="4">
-        <v>42489.71875</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="B20" t="s">
+        <v>143</v>
+      </c>
+      <c r="E20" s="2">
+        <v>4</v>
+      </c>
+      <c r="F20" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>38</v>
+      </c>
+      <c r="B21" t="s">
+        <v>144</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>39</v>
+      </c>
+      <c r="B22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
       </c>
       <c r="E22" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F22" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>36</v>
-      </c>
-      <c r="E23" s="4">
-        <v>42460.333333333336</v>
-      </c>
-      <c r="F23" s="4">
-        <v>42489.40625</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+      <c r="B23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1</v>
+      </c>
+      <c r="F23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>37</v>
-      </c>
-      <c r="E24" s="4">
-        <v>42460.395833333336</v>
-      </c>
-      <c r="F24" s="4">
-        <v>42489.71875</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+      <c r="B24" t="s">
+        <v>59</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>45</v>
+      </c>
+      <c r="B25" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" t="s">
+        <v>60</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26">
-        <v>2</v>
-      </c>
-      <c r="E26" s="2">
-        <v>2</v>
-      </c>
-      <c r="F26" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+      <c r="B26" t="s">
+        <v>145</v>
+      </c>
+      <c r="D26" t="s">
+        <v>61</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>47</v>
+      </c>
+      <c r="B27" t="s">
+        <v>59</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -1327,98 +2718,129 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>41</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E29" s="5"/>
-      <c r="F29" s="4">
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9">
         <v>42489.40625</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E30" s="5"/>
-      <c r="F30" s="4">
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9">
         <v>42489.40625</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E31" s="5"/>
-      <c r="F31" s="4">
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9">
         <v>42489.71875</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>45</v>
-      </c>
-      <c r="D32" t="s">
-        <v>60</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>46</v>
-      </c>
-      <c r="D33" t="s">
-        <v>61</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>47</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34" s="2">
-        <v>1</v>
-      </c>
-      <c r="F34" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>48</v>
-      </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-      <c r="E35" s="2">
-        <v>0</v>
-      </c>
-      <c r="F35" s="2">
-        <v>0</v>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="9"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9">
+        <v>42460.333333333336</v>
+      </c>
+      <c r="F33" s="9">
+        <v>42489.40625</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9">
+        <v>42726.395833333336</v>
+      </c>
+      <c r="F34" s="9">
+        <v>42489.71875</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="9"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9">
+        <v>42460.333333333336</v>
+      </c>
+      <c r="F36" s="9">
+        <v>42489.40625</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9">
+        <v>42460.395833333336</v>
+      </c>
+      <c r="F37" s="9">
+        <v>42489.71875</v>
       </c>
     </row>
   </sheetData>
@@ -1430,33 +2852,35 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E35" sqref="A10:E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="10"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="8"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -1466,108 +2890,135 @@
       <c r="C2" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="11"/>
+      <c r="E2" s="18"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
       <c r="D3">
         <v>533463</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="4">
         <v>533582</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>87</v>
       </c>
-      <c r="E4" s="7"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
       <c r="D5" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
+      <c r="B6" t="s">
+        <v>59</v>
+      </c>
       <c r="D6">
         <v>2015</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="4">
         <v>2015</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
+      <c r="B7" t="s">
+        <v>59</v>
+      </c>
       <c r="D7" t="s">
         <v>65</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
       <c r="D8" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
+      <c r="B9" t="s">
+        <v>59</v>
+      </c>
       <c r="D9" t="s">
         <v>100</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
+      <c r="B10" t="s">
+        <v>140</v>
+      </c>
       <c r="D10" t="s">
         <v>101</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="6" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
+      <c r="B11" t="s">
+        <v>146</v>
+      </c>
       <c r="D11" t="s">
         <v>102</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="6" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -1580,66 +3031,81 @@
       <c r="D12">
         <v>42068.583333333336</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="7">
         <v>42068.333333333336</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>34</v>
       </c>
+      <c r="B13" t="s">
+        <v>59</v>
+      </c>
       <c r="D13" t="s">
         <v>73</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>29</v>
       </c>
+      <c r="B14" t="s">
+        <v>147</v>
+      </c>
       <c r="D14" t="s">
         <v>65</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="6" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>88</v>
       </c>
+      <c r="B15" t="s">
+        <v>59</v>
+      </c>
       <c r="D15">
         <v>2</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>40</v>
       </c>
+      <c r="B16" t="s">
+        <v>59</v>
+      </c>
       <c r="D16">
         <v>1</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>31</v>
       </c>
+      <c r="B17" t="s">
+        <v>142</v>
+      </c>
       <c r="D17" t="s">
         <v>65</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="6" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>89</v>
       </c>
@@ -1652,44 +3118,50 @@
       <c r="D18">
         <v>42299.583333333336</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="7">
         <v>42285.333333333336</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>90</v>
       </c>
+      <c r="B19" t="s">
+        <v>148</v>
+      </c>
       <c r="D19" t="s">
         <v>103</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="6" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>46</v>
       </c>
+      <c r="B20" t="s">
+        <v>145</v>
+      </c>
       <c r="D20" t="s">
         <v>76</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="6" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>91</v>
       </c>
       <c r="D21" t="s">
         <v>65</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="6" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>92</v>
       </c>
@@ -1702,11 +3174,11 @@
       <c r="D22">
         <v>42297.729166666664</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E22" s="7">
         <v>42286.333333333336</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>93</v>
       </c>
@@ -1719,22 +3191,22 @@
       <c r="D23">
         <v>42297.729166666664</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="7">
         <v>42286.333333333336</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>94</v>
       </c>
       <c r="D24">
         <v>2</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>95</v>
       </c>
@@ -1747,83 +3219,95 @@
       <c r="D25" t="s">
         <v>104</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="6" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>96</v>
       </c>
       <c r="D26" t="s">
         <v>65</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>97</v>
       </c>
       <c r="D27" t="s">
         <v>105</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="6" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>98</v>
       </c>
-      <c r="E28" s="7"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E28" s="5"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>1</v>
       </c>
+      <c r="B29" t="s">
+        <v>134</v>
+      </c>
       <c r="D29" t="s">
         <v>106</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="6" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>19</v>
       </c>
+      <c r="B30" t="s">
+        <v>59</v>
+      </c>
       <c r="D30" t="s">
         <v>107</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E30" s="6" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
+      <c r="B31" t="s">
+        <v>59</v>
+      </c>
       <c r="D31" t="s">
         <v>108</v>
       </c>
-      <c r="E31" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E31" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>41</v>
       </c>
+      <c r="B32" t="s">
+        <v>59</v>
+      </c>
       <c r="D32" t="s">
         <v>65</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="E32" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -1836,40 +3320,49 @@
       <c r="D33" t="s">
         <v>109</v>
       </c>
-      <c r="E33" s="8" t="s">
+      <c r="E33" s="6" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>99</v>
       </c>
+      <c r="B34" t="s">
+        <v>149</v>
+      </c>
       <c r="D34" t="s">
         <v>110</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="E34" s="6" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>47</v>
       </c>
+      <c r="B35" t="s">
+        <v>59</v>
+      </c>
       <c r="D35">
         <v>1</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E35" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>48</v>
       </c>
+      <c r="B36" t="s">
+        <v>59</v>
+      </c>
       <c r="D36">
         <v>0</v>
       </c>
-      <c r="E36" s="6">
+      <c r="E36" s="4">
         <v>0</v>
       </c>
     </row>

</xml_diff>